<commit_message>
updated sudoku augmented example
</commit_message>
<xml_diff>
--- a/examples/input_augmented.xlsx
+++ b/examples/input_augmented.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="checks" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="247">
   <si>
     <t xml:space="preserve">genotype</t>
   </si>
@@ -29,6 +29,9 @@
     <t xml:space="preserve">extra</t>
   </si>
   <si>
+    <t xml:space="preserve">pots</t>
+  </si>
+  <si>
     <t xml:space="preserve">check-1</t>
   </si>
   <si>
@@ -45,9 +48,6 @@
   </si>
   <si>
     <t xml:space="preserve">property-c3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pots</t>
   </si>
   <si>
     <t xml:space="preserve">genotype-1</t>
@@ -890,44 +890,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="n">
         <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -948,14 +960,14 @@
   </sheetPr>
   <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="12.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>